<commit_message>
use html templates instead
</commit_message>
<xml_diff>
--- a/filled_invoice.xlsx
+++ b/filled_invoice.xlsx
@@ -136,34 +136,36 @@
     <t>Thank you for your business!</t>
   </si>
   <si>
-    <t>Acme Corp</t>
-  </si>
-  <si>
-    <t>123 Street Address, City, State, Zip</t>
-  </si>
-  <si>
-    <t>www.acmecorp.com, info@acmecorp.com</t>
-  </si>
-  <si>
-    <t>+1234567890</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>Client Company Name</t>
-  </si>
-  <si>
-    <t>Client Address</t>
-  </si>
-  <si>
-    <t>Client Phone, Client Email</t>
-  </si>
-  <si>
-    <t>Jane Doe / Dept</t>
-  </si>
-  <si>
-    <t>Client Phone</t>
+    <t>Wilkinson, Wilkinson and Wilkinson</t>
+  </si>
+  <si>
+    <t>%6961 Britney Meadow
+Lake Willieville, SC 83113-3279, reilly.everett@gmail.com</t>
+  </si>
+  <si>
+    <t>https://uny.com/gjly-gnet.html</t>
+  </si>
+  <si>
+    <t>{0x140004040c0}</t>
+  </si>
+  <si>
+    <t>Mr. Sofia Metz</t>
+  </si>
+  <si>
+    <t>Ziemann and Sons</t>
+  </si>
+  <si>
+    <t>%71 Sadye Light
+Fletatown, KY 53478</t>
+  </si>
+  <si>
+    <t>dillan.nader@rnf.com</t>
+  </si>
+  <si>
+    <t>Murray Marquardt II</t>
+  </si>
+  <si>
+    <t>+18002574390</t>
   </si>
   <si>
     <t>Service Name</t>

</xml_diff>